<commit_message>
ACTUAL PCB: update E. schema, componentenlisjt update.
</commit_message>
<xml_diff>
--- a/ComponentenlijstActualPCB.xlsx
+++ b/ComponentenlijstActualPCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A724989D-CE12-40C3-8F5D-E56D1ADD8D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B055379C-3446-474A-93FD-BCBD5C8FF1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8733DA9E-9F22-460B-BD48-096CF79066EB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Component</t>
   </si>
@@ -56,10 +56,46 @@
     <t>COMPONENTENLIJST ACTUAL PCB</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Phoenix-Contact/1985962?qs=sGAEpiMZZMvZTcaMAxB2AKJ8wpDgQJg5HIMLhg5x2AA%3D</t>
-  </si>
-  <si>
-    <t>1x2 headers</t>
+    <t>2x15</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/econ-connect-female-header-standaard-aantal-rijen-2-aantal-polen-per-rij-15-blg2x15-1-stuks-1492273</t>
+  </si>
+  <si>
+    <t>2x17</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/econ-connect-female-header-standaard-aantal-rijen-2-aantal-polen-per-rij-17-blg2x17-1-stuks-1492276</t>
+  </si>
+  <si>
+    <t>2x10</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/econ-connect-female-header-standaard-aantal-rijen-2-aantal-polen-per-rij-10-blg2x10-1-stuks-1492267</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/econ-connect-female-header-standaard-aantal-rijen-2-aantal-polen-per-rij-8-blg2x8-1-stuks-1492298</t>
+  </si>
+  <si>
+    <t>2x8</t>
+  </si>
+  <si>
+    <t>1x8</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/econ-connect-female-header-standaard-aantal-rijen-1-aantal-polen-per-rij-8-blg1x8-1-stuks-1492302</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Phoenix-Contact/1714955?qs=sGAEpiMZZMvZTcaMAxB2AKJ8wpDgQJg56QuuQcQ95jA%3D</t>
+  </si>
+  <si>
+    <t>1x2 headers 30 A</t>
+  </si>
+  <si>
+    <t>1x2 headers 15 A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/CUI-Devices/TB002-500-02BE?qs=sGAEpiMZZMvZTcaMAxB2AHpdXjUJWjdtGYWJDK8ID%2FsZJpc5bbOw%2FQ%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -444,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D078FBA-0249-4A49-9B31-EC45C35062C4}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -482,10 +518,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
-        <v>1.36</v>
+        <v>1.54</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -494,28 +530,70 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="E7" s="4"/>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
       <c r="B8" s="3"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" s="3"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
       <c r="B10" s="3"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{7BDD5B33-CBDF-49C0-8D1A-F49FB7EA68BA}"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{1A312358-C393-4ED5-AC29-2FA971963DCB}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{955BEA94-EAC1-4A26-9D65-4A1ADACFBC94}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{1F48DF56-F0F8-42F9-9692-0748FEA18D47}"/>
+    <hyperlink ref="E12" r:id="rId4" xr:uid="{73587338-C791-4EF2-8D2F-C3EC2F0A6951}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Planning over alle componenten. bord desgin voor de relais getekend op CAD.
</commit_message>
<xml_diff>
--- a/ComponentenlijstActualPCB.xlsx
+++ b/ComponentenlijstActualPCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B055379C-3446-474A-93FD-BCBD5C8FF1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408AC441-A3A7-424F-BA06-4D858A11D2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8733DA9E-9F22-460B-BD48-096CF79066EB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Component</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/CUI-Devices/TB002-500-02BE?qs=sGAEpiMZZMvZTcaMAxB2AHpdXjUJWjdtGYWJDK8ID%2FsZJpc5bbOw%2FQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://nl.rs-online.com/web/p/heatsinks/1898628/</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D078FBA-0249-4A49-9B31-EC45C35062C4}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,12 +591,18 @@
         <v>20</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1" xr:uid="{1A312358-C393-4ED5-AC29-2FA971963DCB}"/>
     <hyperlink ref="E11" r:id="rId2" xr:uid="{955BEA94-EAC1-4A26-9D65-4A1ADACFBC94}"/>
     <hyperlink ref="E6" r:id="rId3" xr:uid="{1F48DF56-F0F8-42F9-9692-0748FEA18D47}"/>
     <hyperlink ref="E12" r:id="rId4" xr:uid="{73587338-C791-4EF2-8D2F-C3EC2F0A6951}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{29C3ADEF-E2EF-416D-8A4D-877AF8612729}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>